<commit_message>
Completed Baseline judgmental forecasting analysis
</commit_message>
<xml_diff>
--- a/0_0_Data/2_Processed_Data/2_GDP_Evaluation_series/first_release_qoq_GDP.xlsx
+++ b/0_0_Data/2_Processed_Data/2_GDP_Evaluation_series/first_release_qoq_GDP.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dfbe04e23282f0d1/Desktop/ifo/Konjunkturprognose Evaluierung/ifo Forecast Evaluation Workfolder/0_0_Data/2_Processed_Data/2_GDP_Evaluation_series/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_5365C631A46093250EFE31D2F87AE380788FAB3A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{771871EF-9995-461B-A31B-B6DB525E1489}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-14505" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -25,11 +31,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,17 +97,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -139,7 +153,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -173,6 +187,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -207,9 +222,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -382,14 +398,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="32.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -397,7 +416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>32370</v>
       </c>
@@ -405,39 +424,39 @@
         <v>1.098540744384322</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>32462</v>
       </c>
       <c r="B3">
-        <v>1.200129743756077</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>1.2001297437560769</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>32554</v>
       </c>
       <c r="B4">
-        <v>1.025641025641019</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>1.0256410256410191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>32643</v>
       </c>
       <c r="B5">
-        <v>0.4124365482233615</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>0.41243654822336151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>32735</v>
       </c>
       <c r="B6">
-        <v>0.9004739336492845</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>0.90047393364928452</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>32827</v>
       </c>
@@ -445,71 +464,71 @@
         <v>1.174260216063898</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>32919</v>
       </c>
       <c r="B8">
-        <v>2.073661405137701</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>2.0736614051377011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>33008</v>
       </c>
       <c r="B9">
-        <v>0.4851425106125105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>0.48514251061251051</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>33100</v>
       </c>
       <c r="B10">
-        <v>2.11225105612553</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>2.1122510561255301</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>33192</v>
       </c>
       <c r="B11">
-        <v>1.773049645390049</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>1.7730496453900491</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>33284</v>
       </c>
       <c r="B12">
-        <v>2.758420441347291</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>2.7584204413472908</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>33373</v>
       </c>
       <c r="B13">
-        <v>1.113617141246129</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>1.1136171412461291</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>33465</v>
       </c>
       <c r="B14">
-        <v>-0.5994702356057567</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>-0.59947023560575674</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>33557</v>
       </c>
       <c r="B15">
-        <v>0.8695652173913095</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>0.86956521739130954</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>33649</v>
       </c>
@@ -517,31 +536,31 @@
         <v>1.348720800889869</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>33739</v>
       </c>
       <c r="B17">
-        <v>-0.04115790917821152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>-4.1157909178211521E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>33831</v>
       </c>
       <c r="B18">
-        <v>-0.1509744715893349</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>-0.15097447158933491</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>33923</v>
       </c>
       <c r="B19">
-        <v>-0.1374570446735577</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>-0.13745704467355771</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>34015</v>
       </c>
@@ -549,63 +568,63 @@
         <v>-1.789401238816229</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>34104</v>
       </c>
       <c r="B21">
-        <v>0.6306937631394585</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>0.63069376313945846</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>34196</v>
       </c>
       <c r="B22">
-        <v>0.7242339832868948</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>0.72423398328689481</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>34288</v>
       </c>
       <c r="B23">
-        <v>-0.1935840707964626</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>-0.19358407079646259</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>34380</v>
       </c>
       <c r="B24">
-        <v>1.17761152673871</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>1.1776115267387099</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>34469</v>
       </c>
       <c r="B25">
-        <v>1.232370258797764</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>1.2323702587977641</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>34561</v>
       </c>
       <c r="B26">
-        <v>0.622210198836729</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>0.62221019883672901</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>34653</v>
       </c>
       <c r="B27">
-        <v>0.6183626831563487</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>0.61836268315634868</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>34745</v>
       </c>
@@ -613,39 +632,39 @@
         <v>0.2137608550434148</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>34834</v>
       </c>
       <c r="B29">
-        <v>1.066524463404871</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>1.0665244634048709</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>34926</v>
       </c>
       <c r="B30">
-        <v>-0.01319087191662068</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>-1.319087191662068E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>35018</v>
       </c>
       <c r="B31">
-        <v>-0.4082707757144763</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>-0.40827077571447629</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>35110</v>
       </c>
       <c r="B32">
-        <v>-0.3698811096433335</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>-0.36988110964333348</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>35200</v>
       </c>
@@ -653,31 +672,31 @@
         <v>1.484623541887593</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>35292</v>
       </c>
       <c r="B34">
-        <v>0.8096108644554579</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>0.80961086445545793</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>35384</v>
       </c>
       <c r="B35">
-        <v>0.07776049766718085</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>7.776049766718085E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>35476</v>
       </c>
       <c r="B36">
-        <v>0.4403004403004406</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>0.44030044030044058</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>35565</v>
       </c>
@@ -685,15 +704,15 @@
         <v>1.010493587252234</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>35657</v>
       </c>
       <c r="B38">
-        <v>0.782251859451141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>0.78225185945114095</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>35749</v>
       </c>
@@ -701,15 +720,15 @@
         <v>0.280183392766165</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>35841</v>
       </c>
       <c r="B40">
-        <v>0.9522600304723229</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>0.95226003047232288</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>35930</v>
       </c>
@@ -717,55 +736,55 @@
         <v>0.1008191556395778</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>36022</v>
       </c>
       <c r="B42">
-        <v>0.8692365835223037</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>0.86923658352230371</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>36114</v>
       </c>
       <c r="B43">
-        <v>-0.3749062734316393</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>-0.37490627343163929</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>36206</v>
       </c>
       <c r="B44">
-        <v>0.4382529163932056</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>0.43825291639320563</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>36295</v>
       </c>
       <c r="B45">
-        <v>0.04238186056368139</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>4.2381860563681387E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>36387</v>
       </c>
       <c r="B46">
-        <v>0.7183604479188681</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>0.71836044791886811</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>36479</v>
       </c>
       <c r="B47">
-        <v>0.6910994764397971</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>0.69109947643979708</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>36571</v>
       </c>
@@ -773,7 +792,7 @@
         <v>0.659619626284904</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>36661</v>
       </c>
@@ -781,55 +800,55 @@
         <v>1.148285832300693</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>36753</v>
       </c>
       <c r="B50">
-        <v>0.5648565427516806</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>0.56485654275168062</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>36845</v>
       </c>
       <c r="B51">
-        <v>0.207068759008509</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>0.20706875900850899</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>36937</v>
       </c>
       <c r="B52">
-        <v>0.3707380320495879</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>0.37073803204958788</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>37026</v>
       </c>
       <c r="B53">
-        <v>-0.03022670025188753</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>-3.022670025188753E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>37118</v>
       </c>
       <c r="B54">
-        <v>-0.1411005845595663</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>-0.14110058455956631</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>37210</v>
       </c>
       <c r="B55">
-        <v>-0.2542372881355935</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>-0.25423728813559349</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>37302</v>
       </c>
@@ -837,31 +856,31 @@
         <v>0.1699235344095065</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>37391</v>
       </c>
       <c r="B57">
-        <v>0.2723861022557598</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
+        <v>0.27238610225575982</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>37483</v>
       </c>
       <c r="B58">
-        <v>0.2679452827527801</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>0.26794528275278012</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>37575</v>
       </c>
       <c r="B59">
-        <v>-0.03213174013455929</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+        <v>-3.2131740134559293E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>37667</v>
       </c>
@@ -869,23 +888,23 @@
         <v>-0.2270033548283337</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>37756</v>
       </c>
       <c r="B61">
-        <v>-0.06231782088652726</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>-6.2317820886527257E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>37848</v>
       </c>
       <c r="B62">
-        <v>0.2194748711340181</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+        <v>0.21947487113401809</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>37940</v>
       </c>
@@ -893,39 +912,39 @@
         <v>0.215019190965168</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>38032</v>
       </c>
       <c r="B64">
-        <v>0.4390009221023837</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
+        <v>0.43900092210238367</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>38122</v>
       </c>
       <c r="B65">
-        <v>0.4754484797634859</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <v>0.47544847976348592</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>38214</v>
       </c>
       <c r="B66">
-        <v>0.09947279419078808</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
+        <v>9.9472794190788083E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>38306</v>
       </c>
       <c r="B67">
-        <v>-0.2327107822662463</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+        <v>-0.23271078226624631</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>38398</v>
       </c>
@@ -933,31 +952,31 @@
         <v>1.04410616705698</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>38487</v>
       </c>
       <c r="B69">
-        <v>0.00970120294917066</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
+        <v>9.7012029491706595E-3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>38579</v>
       </c>
       <c r="B70">
-        <v>0.6204556471158512</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+        <v>0.62045564711585122</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>38671</v>
       </c>
       <c r="B71">
-        <v>0.009625565501978165</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
+        <v>9.6255655019781648E-3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>38763</v>
       </c>
@@ -965,63 +984,63 @@
         <v>0.3653494856263777</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>38852</v>
       </c>
       <c r="B73">
-        <v>0.9010736196319133</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
+        <v>0.90107361963191335</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>38944</v>
       </c>
       <c r="B74">
-        <v>0.6346499952638076</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
+        <v>0.63464999526380761</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>39036</v>
       </c>
       <c r="B75">
-        <v>0.8728296574378289</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
+        <v>0.87282965743782892</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>39128</v>
       </c>
       <c r="B76">
-        <v>0.5106778087279453</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
+        <v>0.51067780872794533</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>39217</v>
       </c>
       <c r="B77">
-        <v>0.2592832669691649</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
+        <v>0.25928326696916493</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>39309</v>
       </c>
       <c r="B78">
-        <v>0.6834764939503178</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
+        <v>0.68347649395031784</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>39401</v>
       </c>
       <c r="B79">
-        <v>0.2660550458715654</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
+        <v>0.26605504587156542</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>39493</v>
       </c>
@@ -1029,63 +1048,63 @@
         <v>1.528044651843707</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>39583</v>
       </c>
       <c r="B81">
-        <v>-0.4957634757526566</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
+        <v>-0.49576347575265661</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>39675</v>
       </c>
       <c r="B82">
-        <v>-0.5244122965641937</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
+        <v>-0.52441229656419375</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>39767</v>
       </c>
       <c r="B83">
-        <v>-2.107941123023812</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+        <v>-2.1079411230238119</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>39859</v>
       </c>
       <c r="B84">
-        <v>-3.800762010965527</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
+        <v>-3.8007620109655269</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>39948</v>
       </c>
       <c r="B85">
-        <v>0.3175214086404294</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
+        <v>0.31752140864042938</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>40040</v>
       </c>
       <c r="B86">
-        <v>0.7280390842034727</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
+        <v>0.72803908420347274</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>40132</v>
       </c>
       <c r="B87">
-        <v>0.009508414947233161</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
+        <v>9.5084149472331615E-3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>40224</v>
       </c>
@@ -1093,31 +1112,31 @@
         <v>0.1613515565679591</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>40313</v>
       </c>
       <c r="B89">
-        <v>2.182091798344627</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
+        <v>2.1820917983446271</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>40405</v>
       </c>
       <c r="B90">
-        <v>0.6980161645848688</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
+        <v>0.69801616458486881</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>40497</v>
       </c>
       <c r="B91">
-        <v>0.3647970816233392</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
+        <v>0.36479708162333918</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>40589</v>
       </c>
@@ -1125,7 +1144,7 @@
         <v>1.499182264219509</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>40678</v>
       </c>
@@ -1133,15 +1152,15 @@
         <v>0.119222303741742</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>40770</v>
       </c>
       <c r="B94">
-        <v>0.5030181086519089</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
+        <v>0.50301810865190888</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>40862</v>
       </c>
@@ -1149,111 +1168,111 @@
         <v>-0.1818677821223996</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>40954</v>
       </c>
       <c r="B96">
-        <v>0.5101576022592715</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2">
+        <v>0.51015760225927154</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>41044</v>
       </c>
       <c r="B97">
-        <v>0.2707092582566427</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2">
+        <v>0.27070925825664272</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>41136</v>
       </c>
       <c r="B98">
-        <v>0.233981281497472</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2">
+        <v>0.23398128149747199</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>41228</v>
       </c>
       <c r="B99">
-        <v>-0.5925127928898435</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2">
+        <v>-0.59251279288984349</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>41320</v>
       </c>
       <c r="B100">
-        <v>0.06328541723172172</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2">
+        <v>6.3285417231721722E-2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>41409</v>
       </c>
       <c r="B101">
-        <v>0.7214356569573426</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2">
+        <v>0.72143565695734257</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>41501</v>
       </c>
       <c r="B102">
-        <v>0.3223207091055595</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2">
+        <v>0.32232070910555949</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>41593</v>
       </c>
       <c r="B103">
-        <v>0.3837572512271369</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2">
+        <v>0.38375725122713689</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>41685</v>
       </c>
       <c r="B104">
-        <v>0.8179231863442404</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2">
+        <v>0.81792318634424044</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105" s="2">
         <v>41774</v>
       </c>
       <c r="B105">
-        <v>-0.1608782057348365</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2">
+        <v>-0.16087820573483649</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A106" s="2">
         <v>41866</v>
       </c>
       <c r="B106">
-        <v>0.06623769871308968</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2">
+        <v>6.6237698713089682E-2</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>41958</v>
       </c>
       <c r="B107">
-        <v>0.6996974281391782</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2">
+        <v>0.69969742813917823</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A108" s="2">
         <v>42050</v>
       </c>
       <c r="B108">
-        <v>0.2723004694835739</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2">
+        <v>0.27230046948357389</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109" s="2">
         <v>42139</v>
       </c>
@@ -1261,103 +1280,103 @@
         <v>0.4386374241717208</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110" s="2">
         <v>42231</v>
       </c>
       <c r="B110">
-        <v>0.315926407730895</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2">
+        <v>0.31592640773089498</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111" s="2">
         <v>42323</v>
       </c>
       <c r="B111">
-        <v>0.2686926711757547</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2">
+        <v>0.26869267117575468</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112" s="2">
         <v>42415</v>
       </c>
       <c r="B112">
-        <v>0.6653114026982063</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2">
+        <v>0.66531140269820632</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113" s="2">
         <v>42505</v>
       </c>
       <c r="B113">
-        <v>0.4112593675744862</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2">
+        <v>0.41125936757448622</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114" s="2">
         <v>42597</v>
       </c>
       <c r="B114">
-        <v>0.1911349777009136</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2">
+        <v>0.19113497770091359</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A115" s="2">
         <v>42689</v>
       </c>
       <c r="B115">
-        <v>0.4269234262875818</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2">
+        <v>0.42692342628758179</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A116" s="2">
         <v>42781</v>
       </c>
       <c r="B116">
-        <v>0.6058961837583665</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2">
+        <v>0.60589618375836651</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117" s="2">
         <v>42870</v>
       </c>
       <c r="B117">
-        <v>0.6164567140176875</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2">
+        <v>0.61645671401768753</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A118" s="2">
         <v>42962</v>
       </c>
       <c r="B118">
-        <v>0.8241758241758176</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2">
+        <v>0.82417582417581758</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A119" s="2">
         <v>43054</v>
       </c>
       <c r="B119">
-        <v>0.6069669247009128</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2">
+        <v>0.60696692470091285</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A120" s="2">
         <v>43146</v>
       </c>
       <c r="B120">
-        <v>0.2972807554428514</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2">
+        <v>0.29728075544285137</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121" s="2">
         <v>43235</v>
       </c>
       <c r="B121">
-        <v>0.4515848892748554</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2">
+        <v>0.45158488927485541</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122" s="2">
         <v>43327</v>
       </c>
@@ -1365,87 +1384,87 @@
         <v>-0.1988415319443278</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123" s="2">
         <v>43419</v>
       </c>
       <c r="B123">
-        <v>0.01732351667388135</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2">
+        <v>1.7323516673881351E-2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A124" s="2">
         <v>43511</v>
       </c>
       <c r="B124">
-        <v>0.4243526457088377</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2">
+        <v>0.42435264570883768</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A125" s="2">
         <v>43600</v>
       </c>
       <c r="B125">
-        <v>-0.07468957146858211</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2">
+        <v>-7.4689571468582114E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126" s="2">
         <v>43692</v>
       </c>
       <c r="B126">
-        <v>0.08415934168693044</v>
-      </c>
-    </row>
-    <row r="127" spans="1:2">
+        <v>8.4159341686930442E-2</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A127" s="2">
         <v>43784</v>
       </c>
       <c r="B127">
-        <v>0.02799552071668639</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2">
+        <v>2.799552071668639E-2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128" s="2">
         <v>43876</v>
       </c>
       <c r="B128">
-        <v>-2.221807318894706</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2">
+        <v>-2.2218073188947058</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A129" s="2">
         <v>43966</v>
       </c>
       <c r="B129">
-        <v>-9.690957649751999</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2">
+        <v>-9.6909576497519989</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A130" s="2">
         <v>44058</v>
       </c>
       <c r="B130">
-        <v>8.48030415038547</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2">
+        <v>8.4803041503854697</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A131" s="2">
         <v>44150</v>
       </c>
       <c r="B131">
-        <v>0.3406326034063205</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2">
+        <v>0.34063260340632051</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132" s="2">
         <v>44242</v>
       </c>
       <c r="B132">
-        <v>-1.806937868393072</v>
-      </c>
-    </row>
-    <row r="133" spans="1:2">
+        <v>-1.8069378683930719</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A133" s="2">
         <v>44331</v>
       </c>
@@ -1453,7 +1472,7 @@
         <v>1.633092118130258</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A134" s="2">
         <v>44423</v>
       </c>
@@ -1461,23 +1480,23 @@
         <v>1.694266296544459</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A135" s="2">
         <v>44515</v>
       </c>
       <c r="B135">
-        <v>-0.3471896406117954</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2">
+        <v>-0.34718964061179541</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136" s="2">
         <v>44607</v>
       </c>
       <c r="B136">
-        <v>0.2354048964218456</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2">
+        <v>0.23540489642184559</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137" s="2">
         <v>44696</v>
       </c>
@@ -1485,23 +1504,23 @@
         <v>0.1397298556124878</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138" s="2">
         <v>44788</v>
       </c>
       <c r="B138">
-        <v>0.4001488926112106</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2">
+        <v>0.40014889261121062</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139" s="2">
         <v>44880</v>
       </c>
       <c r="B139">
-        <v>-0.4353061035472806</v>
-      </c>
-    </row>
-    <row r="140" spans="1:2">
+        <v>-0.43530610354728061</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140" s="2">
         <v>44972</v>
       </c>
@@ -1509,15 +1528,15 @@
         <v>-0.3352267436446591</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141" s="2">
         <v>45061</v>
       </c>
       <c r="B141">
-        <v>0.01855976243503714</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2">
+        <v>1.8559762435037139E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A142" s="2">
         <v>45153</v>
       </c>
@@ -1525,63 +1544,63 @@
         <v>-0.1296176279974082</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143" s="2">
         <v>45245</v>
       </c>
       <c r="B143">
-        <v>-0.2870636170015632</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2">
+        <v>-0.28706361700156319</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144" s="2">
         <v>45337</v>
       </c>
       <c r="B144">
-        <v>0.2135958395245076</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2">
+        <v>0.21359583952450761</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A145" s="2">
         <v>45427</v>
       </c>
       <c r="B145">
-        <v>-0.06676204101096155</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2">
+        <v>-6.6762041010961545E-2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A146" s="2">
         <v>45519</v>
       </c>
       <c r="B146">
-        <v>0.1052128168340501</v>
-      </c>
-    </row>
-    <row r="147" spans="1:2">
+        <v>0.10521281683405009</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147" s="2">
         <v>45611</v>
       </c>
       <c r="B147">
-        <v>-0.2006497229122814</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2">
+        <v>-0.20064972291228139</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A148" s="2">
         <v>45703</v>
       </c>
       <c r="B148">
-        <v>0.4116802297750048</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2">
+        <v>0.41168022977500479</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149" s="2">
         <v>45792</v>
       </c>
       <c r="B149">
-        <v>-0.2766911554241067</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2">
+        <v>-0.27669115542410672</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150" s="2">
         <v>45884</v>
       </c>

</xml_diff>